<commit_message>
generating spreadsheet for a released TKID dark array
</commit_message>
<xml_diff>
--- a/masks/code/antenna_coupled_TKIDs_20190214_modified.xlsx
+++ b/masks/code/antenna_coupled_TKIDs_20190214_modified.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Patches" sheetId="1" r:id="rId1"/>
     <sheet name="Shift_Calculator" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="153">
   <si>
     <t>AGA Marks</t>
   </si>
@@ -473,6 +473,21 @@
   <si>
     <t>Also delete C1R1, C3R1, C2R2, C4R2</t>
   </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
 </sst>
 </file>
 
@@ -505,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -539,11 +554,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,6 +607,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="W61" sqref="W61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,14 +1251,14 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="8" t="s">
+      <c r="T12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
       <c r="Z12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1217,46 +1268,46 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="8" t="s">
+      <c r="N13" s="11"/>
+      <c r="O13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="P13" s="11"/>
       <c r="Q13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="8" t="s">
+      <c r="T13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="9"/>
-      <c r="V13" s="8" t="s">
+      <c r="U13" s="11"/>
+      <c r="V13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W13" s="9"/>
-      <c r="X13" s="8" t="s">
+      <c r="W13" s="11"/>
+      <c r="X13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="9"/>
+      <c r="Y13" s="11"/>
       <c r="Z13" s="4" t="s">
         <v>18</v>
       </c>
@@ -4314,79 +4365,79 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="1">
-        <v>-3.5345</v>
-      </c>
-      <c r="E55" s="1">
+      <c r="D55" s="8">
+        <v>-3.5339999999999998</v>
+      </c>
+      <c r="E55" s="8">
         <v>-7.1970000000000001</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="8">
         <v>6.8</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="8">
         <v>1.8</v>
       </c>
-      <c r="H55" s="1">
-        <v>-6.9344999999999999</v>
-      </c>
-      <c r="I55" s="1">
-        <v>-0.13450000000000009</v>
-      </c>
-      <c r="J55" s="1">
+      <c r="H55" s="8">
+        <v>-6.9339999999999993</v>
+      </c>
+      <c r="I55" s="8">
+        <v>-0.1339999999999999</v>
+      </c>
+      <c r="J55" s="8">
         <v>-6.2969999999999997</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="8">
         <v>-8.0969999999999995</v>
       </c>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1">
-        <v>0</v>
-      </c>
-      <c r="N55" s="1">
+      <c r="L55" s="8"/>
+      <c r="M55" s="8">
+        <v>0</v>
+      </c>
+      <c r="N55" s="8">
         <v>-4.944</v>
       </c>
-      <c r="O55" s="1">
-        <v>-3.5345</v>
-      </c>
-      <c r="P55" s="1">
+      <c r="O55" s="8">
+        <v>-3.5339999999999998</v>
+      </c>
+      <c r="P55" s="8">
         <v>-2.2530000000000001</v>
       </c>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1" t="s">
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="T55" s="1">
+      <c r="T55" s="8">
         <v>6</v>
       </c>
-      <c r="U55" s="1">
+      <c r="U55" s="8">
         <v>6</v>
       </c>
-      <c r="V55" s="1">
-        <v>0</v>
-      </c>
-      <c r="W55" s="1">
+      <c r="V55" s="8">
+        <v>0</v>
+      </c>
+      <c r="W55" s="8">
         <v>5.8360000000000003</v>
       </c>
-      <c r="X55" s="1">
+      <c r="X55" s="8">
         <v>8.7539999999999996</v>
       </c>
-      <c r="Y55" s="1">
+      <c r="Y55" s="8">
         <v>11.672000000000001</v>
       </c>
-      <c r="Z55" s="1" t="s">
+      <c r="Z55" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AA55" s="1"/>
-      <c r="AB55" s="1"/>
+      <c r="AA55" s="8"/>
+      <c r="AB55" s="8"/>
     </row>
     <row r="56" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
@@ -4721,13 +4772,14 @@
         <v>0</v>
       </c>
       <c r="N60" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="O60" s="1">
         <v>-0.47499999999999998</v>
       </c>
       <c r="P60" s="1">
-        <v>0.27500000000000002</v>
+        <f>E60-N60</f>
+        <v>-0.125</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -4744,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="W60" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="X60" s="1">
         <v>8.7539999999999996</v>
@@ -9976,10 +10028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA500"/>
+  <dimension ref="A1:AA503"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10010,18 +10062,18 @@
         <v>126</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="11"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
         <v>118</v>
@@ -12235,63 +12287,63 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="1"/>
-      <c r="AA55" s="1"/>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="1"/>
-      <c r="W56" s="1"/>
-      <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="1"/>
-      <c r="AA56" s="1"/>
+    <row r="55" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="8"/>
+      <c r="W55" s="8"/>
+      <c r="X55" s="8"/>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="8"/>
+    </row>
+    <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="8"/>
+      <c r="X56" s="8"/>
+      <c r="Y56" s="8"/>
+      <c r="Z56" s="8"/>
+      <c r="AA56" s="8"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -12322,37 +12374,43 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
-      <c r="W58" s="1"/>
-      <c r="X58" s="1"/>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="1"/>
-      <c r="AA58" s="1"/>
+    <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="M58" s="13"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="8"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="2"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -12361,10 +12419,18 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
+      <c r="J59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
@@ -12381,19 +12447,43 @@
       <c r="AA59" s="1"/>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="A60" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="8">
+        <v>6</v>
+      </c>
+      <c r="D60" s="8">
+        <v>6</v>
+      </c>
+      <c r="E60" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="F60" s="8">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G60" s="8">
+        <v>8.7539999999999996</v>
+      </c>
+      <c r="H60" s="8">
+        <v>11.672000000000001</v>
+      </c>
       <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
+      <c r="J60" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L60" s="8">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="M60" s="8">
+        <v>0</v>
+      </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -12419,10 +12509,18 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
+      <c r="J61" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L61" s="8">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="M61" s="8">
+        <v>0</v>
+      </c>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -12448,10 +12546,18 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
+      <c r="J62" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L62" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="M62" s="8">
+        <v>0</v>
+      </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -12477,10 +12583,18 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
+      <c r="J63" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L63" s="8">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="M63" s="8">
+        <v>0</v>
+      </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -12506,10 +12620,18 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
+      <c r="J64" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L64" s="8">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="M64" s="8">
+        <v>0</v>
+      </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -12535,10 +12657,18 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
+      <c r="J65" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L65" s="8">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="M65" s="8">
+        <v>0</v>
+      </c>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -12578,10 +12708,6 @@
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
-      <c r="X66" s="1"/>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="1"/>
-      <c r="AA66" s="1"/>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
@@ -12607,25 +12733,45 @@
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+      <c r="A68" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="8">
+        <v>6</v>
+      </c>
+      <c r="D68" s="8">
+        <v>6</v>
+      </c>
+      <c r="E68" s="8">
+        <v>-2.1</v>
+      </c>
+      <c r="F68" s="8">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G68" s="8">
+        <v>8.7539999999999996</v>
+      </c>
+      <c r="H68" s="8">
+        <v>11.672000000000001</v>
+      </c>
       <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
+      <c r="J68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L68" s="1">
+        <v>-0.57199999999999995</v>
+      </c>
+      <c r="M68" s="1">
+        <v>0</v>
+      </c>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
@@ -12636,10 +12782,6 @@
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
@@ -12651,10 +12793,18 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
+      <c r="J69" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L69" s="1">
+        <v>-0.48399999999999999</v>
+      </c>
+      <c r="M69" s="8">
+        <v>0</v>
+      </c>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -12665,10 +12815,6 @@
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
@@ -12680,10 +12826,18 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
+      <c r="J70" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L70" s="1">
+        <v>-0.77200000000000002</v>
+      </c>
+      <c r="M70" s="8">
+        <v>0</v>
+      </c>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -12694,10 +12848,6 @@
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-      <c r="AA70" s="1"/>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -12709,10 +12859,18 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="J71" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L71" s="1">
+        <v>-0.66800000000000004</v>
+      </c>
+      <c r="M71" s="8">
+        <v>0</v>
+      </c>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -12723,10 +12881,6 @@
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="1"/>
-      <c r="AA71" s="1"/>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
@@ -12738,10 +12892,18 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
+      <c r="J72" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K72" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L72" s="1">
+        <v>-1.016</v>
+      </c>
+      <c r="M72" s="8">
+        <v>0</v>
+      </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -12767,10 +12929,18 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
+      <c r="J73" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K73" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L73" s="1">
+        <v>-0.88800000000000001</v>
+      </c>
+      <c r="M73" s="8">
+        <v>0</v>
+      </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -12845,19 +13015,43 @@
       <c r="AA75" s="1"/>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
+      <c r="A76" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="8">
+        <v>6</v>
+      </c>
+      <c r="D76" s="8">
+        <v>6</v>
+      </c>
+      <c r="E76" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="F76" s="8">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G76" s="8">
+        <v>8.7539999999999996</v>
+      </c>
+      <c r="H76" s="8">
+        <v>11.672000000000001</v>
+      </c>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K76" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L76" s="8">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="M76" s="8">
+        <v>0.47199999999999998</v>
+      </c>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
@@ -12874,19 +13068,27 @@
       <c r="AA76" s="1"/>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K77" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L77" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="M77" s="8">
+        <v>0.497</v>
+      </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
@@ -12903,19 +13105,27 @@
       <c r="AA77" s="1"/>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K78" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L78" s="8">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="M78" s="8">
+        <v>-0.45300000000000001</v>
+      </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
@@ -12932,19 +13142,27 @@
       <c r="AA78" s="1"/>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K79" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L79" s="8">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="M79" s="8">
+        <v>0.46800000000000003</v>
+      </c>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
@@ -12961,19 +13179,27 @@
       <c r="AA79" s="1"/>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K80" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L80" s="8">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="M80" s="8">
+        <v>-0.32500000000000001</v>
+      </c>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
@@ -12990,19 +13216,27 @@
       <c r="AA80" s="1"/>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K81" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L81" s="8">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="M81" s="8">
+        <v>-6.2E-2</v>
+      </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
@@ -13019,19 +13253,19 @@
       <c r="AA81" s="1"/>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="8"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -13048,19 +13282,19 @@
       <c r="AA82" s="1"/>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
@@ -13077,19 +13311,43 @@
       <c r="AA83" s="1"/>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
+      <c r="A84" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="8">
+        <v>6</v>
+      </c>
+      <c r="D84" s="8">
+        <v>6</v>
+      </c>
+      <c r="E84" s="8">
+        <v>-2.1</v>
+      </c>
+      <c r="F84" s="8">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G84" s="8">
+        <v>8.7539999999999996</v>
+      </c>
+      <c r="H84" s="8">
+        <v>11.672000000000001</v>
+      </c>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K84" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L84" s="8">
+        <v>-0.56799999999999995</v>
+      </c>
+      <c r="M84" s="8">
+        <v>0.25600000000000001</v>
+      </c>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
@@ -13106,19 +13364,27 @@
       <c r="AA84" s="1"/>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K85" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L85" s="8">
+        <v>-0.48</v>
+      </c>
+      <c r="M85" s="8">
+        <v>0.20799999999999999</v>
+      </c>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -13135,19 +13401,27 @@
       <c r="AA85" s="1"/>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K86" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L86" s="8">
+        <v>-0.76800000000000002</v>
+      </c>
+      <c r="M86" s="8">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
@@ -13164,19 +13438,27 @@
       <c r="AA86" s="1"/>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K87" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L87" s="8">
+        <v>-0.66400000000000003</v>
+      </c>
+      <c r="M87" s="8">
+        <v>0.27900000000000003</v>
+      </c>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
@@ -13193,19 +13475,27 @@
       <c r="AA87" s="1"/>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
-      <c r="M88" s="1"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K88" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L88" s="8">
+        <v>1.012</v>
+      </c>
+      <c r="M88" s="8">
+        <v>-0.40200000000000002</v>
+      </c>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
@@ -13222,19 +13512,27 @@
       <c r="AA88" s="1"/>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K89" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L89" s="8">
+        <v>-0.88400000000000001</v>
+      </c>
+      <c r="M89" s="8">
+        <v>-0.17499999999999999</v>
+      </c>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
@@ -25169,11 +25467,99 @@
       <c r="Z500" s="1"/>
       <c r="AA500" s="1"/>
     </row>
+    <row r="501" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A501" s="1"/>
+      <c r="B501" s="1"/>
+      <c r="C501" s="1"/>
+      <c r="D501" s="1"/>
+      <c r="E501" s="1"/>
+      <c r="F501" s="1"/>
+      <c r="G501" s="1"/>
+      <c r="H501" s="1"/>
+      <c r="I501" s="1"/>
+      <c r="J501" s="1"/>
+      <c r="K501" s="1"/>
+      <c r="L501" s="1"/>
+      <c r="M501" s="1"/>
+      <c r="N501" s="1"/>
+      <c r="O501" s="1"/>
+      <c r="P501" s="1"/>
+      <c r="Q501" s="1"/>
+      <c r="R501" s="1"/>
+      <c r="S501" s="1"/>
+      <c r="T501" s="1"/>
+      <c r="U501" s="1"/>
+      <c r="V501" s="1"/>
+      <c r="W501" s="1"/>
+      <c r="X501" s="1"/>
+      <c r="Y501" s="1"/>
+      <c r="Z501" s="1"/>
+      <c r="AA501" s="1"/>
+    </row>
+    <row r="502" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A502" s="1"/>
+      <c r="B502" s="1"/>
+      <c r="C502" s="1"/>
+      <c r="D502" s="1"/>
+      <c r="E502" s="1"/>
+      <c r="F502" s="1"/>
+      <c r="G502" s="1"/>
+      <c r="H502" s="1"/>
+      <c r="I502" s="1"/>
+      <c r="J502" s="1"/>
+      <c r="K502" s="1"/>
+      <c r="L502" s="1"/>
+      <c r="M502" s="1"/>
+      <c r="N502" s="1"/>
+      <c r="O502" s="1"/>
+      <c r="P502" s="1"/>
+      <c r="Q502" s="1"/>
+      <c r="R502" s="1"/>
+      <c r="S502" s="1"/>
+      <c r="T502" s="1"/>
+      <c r="U502" s="1"/>
+      <c r="V502" s="1"/>
+      <c r="W502" s="1"/>
+      <c r="X502" s="1"/>
+      <c r="Y502" s="1"/>
+      <c r="Z502" s="1"/>
+      <c r="AA502" s="1"/>
+    </row>
+    <row r="503" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A503" s="1"/>
+      <c r="B503" s="1"/>
+      <c r="C503" s="1"/>
+      <c r="D503" s="1"/>
+      <c r="E503" s="1"/>
+      <c r="F503" s="1"/>
+      <c r="G503" s="1"/>
+      <c r="H503" s="1"/>
+      <c r="I503" s="1"/>
+      <c r="J503" s="1"/>
+      <c r="K503" s="1"/>
+      <c r="L503" s="1"/>
+      <c r="M503" s="1"/>
+      <c r="N503" s="1"/>
+      <c r="O503" s="1"/>
+      <c r="P503" s="1"/>
+      <c r="Q503" s="1"/>
+      <c r="R503" s="1"/>
+      <c r="S503" s="1"/>
+      <c r="T503" s="1"/>
+      <c r="U503" s="1"/>
+      <c r="V503" s="1"/>
+      <c r="W503" s="1"/>
+      <c r="X503" s="1"/>
+      <c r="Y503" s="1"/>
+      <c r="Z503" s="1"/>
+      <c r="AA503" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="L58:M58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>